<commit_message>
Added Python 3 Quiz Hard
</commit_message>
<xml_diff>
--- a/quizzes.xlsx
+++ b/quizzes.xlsx
@@ -9,11 +9,12 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Web Development 1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Cryptography 1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Python 1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="General 2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="General Easy 1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="General 3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Python 1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="General 2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="General Easy 1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="General 3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Cryptography 1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Python 3" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -773,342 +774,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Cryptography 1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Cryptography</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>What does “encryption” do to data?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Deletes it</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Compresses it</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Makes it unreadable without a key</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sends it faster</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>What is the opposite of encryption?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Translation</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Decryption</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Compilation</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Which one is a symmetric key algorithm?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>RSA</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>AES</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ECC</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>DSA</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>What is a hash function primarily used for?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Encryption</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Compression</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Data integrity verification</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Authentication</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Which algorithm is considered broken due to short key length?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>AES</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>DES</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Blowfish</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>RSA-2048</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>What is the size of an SHA-256 hash?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>64 bits</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>128 bits</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>256 bits</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>512 bits</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>What kind of cryptography uses two different keys?</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Symmetric</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Asymmetric</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Elliptic</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Hashing</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>What does a digital signature ensure?</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Faster loading</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Data authenticity and integrity</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Confidentiality only</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Compression of data</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>What is “salting” in password hashing?</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Encrypting passwords</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Adding a secret value before hashing to prevent rainbow table attacks</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Encoding data into Base64</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Decrypting a stored password</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Which algorithm is commonly used in blockchain for proof-of-work?</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RSA</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>MD5</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>SHA-256</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>HMAC</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1415,7 +1080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1601,7 +1266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1869,6 +1534,222 @@
         </is>
       </c>
       <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>General 3</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>A directory</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>An access code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>How many bits is a byte?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>How do you subscribe to an Internet mailing list?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Contact your Internet service provider</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Send e-mail to the list manager</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Telephone the mailing list webmaster</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Send a letter to the list</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Computers calculate numbers in what mode?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Decimal</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Octal</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Binary</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>None of the above</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>What is an FET?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Farad Effect Transformer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Field Effect Transformer</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Field Effect Transistor</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>French Energy Transfer</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The speed of your net access is defined in terms of...</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MHz</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Kbps</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Megabytes</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>How many diodes are in a full wave bridge rectifier?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1894,74 +1775,74 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>General 3</t>
+          <t>Cryptography 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Highlight</t>
+          <t>Translation</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Clip art</t>
+          <t>Decryption</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>What's a web browser?</t>
+          <t>Which one is a symmetric key algorithm?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A kind of spider</t>
+          <t>RSA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A computer that stores WWW files</t>
+          <t>AES</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>A person who likes to look at websites</t>
+          <t>ECC</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>A software program that allows you to access sites on the World Wide Web</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://github.com - is an example of what?</t>
+          <t>What is a hash function primarily used for?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A directory</t>
+          <t>Encryption</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>An access code</t>
+          <t>Compression</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>A URL</t>
+          <t>Data integrity verification</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A server</t>
+          <t>Authentication</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -1971,27 +1852,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>How many bits is a byte?</t>
+          <t>Which algorithm is considered broken due to short key length?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>AES</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>DES</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>Blowfish</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>RSA-2048</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -2001,57 +1882,333 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>How do you subscribe to an Internet mailing list?</t>
+          <t>What is the size of an SHA-256 hash?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Contact your Internet service provider</t>
+          <t>64 bits</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Send e-mail to the list manager</t>
+          <t>128 bits</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Telephone the mailing list webmaster</t>
+          <t>256 bits</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Send a letter to the list</t>
+          <t>512 bits</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Computers calculate numbers in what mode?</t>
+          <t>What kind of cryptography uses two different keys?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Decimal</t>
+          <t>Symmetric</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Octal</t>
+          <t>Asymmetric</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Binary</t>
+          <t>Elliptic</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>None of the above</t>
+          <t>Hashing</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>What does a digital signature ensure?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Faster loading</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Data authenticity and integrity</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Confidentiality only</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Compression of data</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>What is “salting” in password hashing?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Encrypting passwords</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Adding a secret value before hashing to prevent rainbow table attacks</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Encoding data into Base64</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Decrypting a stored password</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Which algorithm is commonly used in blockchain for proof-of-work?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RSA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MD5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>SHA-256</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>HMAC</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Python 3</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What does the @classmethod decorator do?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Converts a method into a static method</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Converts a method so it can only be called on class instances</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Converts a method to receive the class as the first argument instead of the instance</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Makes the method private</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Which of the following statements is TRUE about Python’s GIL (Global Interpreter Lock)?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>It allows true parallel execution of threads on multiple CPUs</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>It prevents memory leaks in C extensions</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>It ensures only one thread executes Python bytecode at a time</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>It is removed in Python 3.10</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>How can you create a custom context manager in Python?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Using @classmethod</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Using __init__ and __del__</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>By defining __enter__ and __exit__ methods</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>By using yield without any decorators</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Which of the following is used to define an abstract method in Python?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>from abc import abstractmethod</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>@abstractmethod</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>def method(self): pass</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Both A and B</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>What is the primary purpose of __slots__ in a class?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>To define class-level constants</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>To create a dictionary for instance variables</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>To prevent dynamic creation of new attributes and reduce memory</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>To define abstract methods</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -2061,57 +2218,57 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>What is an FET?</t>
+          <t>Which statement is true about Python descriptors?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Farad Effect Transformer</t>
+          <t>They only work with class methods</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Field Effect Transformer</t>
+          <t>They define attribute access using __get__, __set__, __delete__</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Field Effect Transistor</t>
+          <t>Descriptors are only available in Python 3.10+</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>French Energy Transfer</t>
+          <t>Descriptors cannot be reused across classes</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>The speed of your net access is defined in terms of...</t>
+          <t>What is a coroutine in Python?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RAM</t>
+          <t>A thread</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MHz</t>
+          <t>A class with __iter__</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Kbps</t>
+          <t>a function paused with yield and resumed later</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Megabytes</t>
+          <t>A method in a metaclass</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -2121,31 +2278,91 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>How many diodes are in a full wave bridge rectifier?</t>
+          <t>Which of the following is not a valid use of a metaclass?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Injecting methods into a class</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Enforcing naming conventions</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Changing inheritance at runtime</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Dynamically creating instance variables</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>What does weakref module provide in Python?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Multithreading support</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>References that do not increase reference count</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Dynamic type checking</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Object pooling</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>What does the super() function do in Python?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Calls a method from a subclass</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Calls the next method in the method resolution order (MRO)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Creates a static method</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Returns the parent class constructor  directly</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Web Development 3
</commit_message>
<xml_diff>
--- a/quizzes.xlsx
+++ b/quizzes.xlsx
@@ -15,6 +15,7 @@
     <sheet name="General 3" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Cryptography 1" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Python 3" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Web Development 3" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2368,4 +2369,340 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Web Development 3</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Web Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What does the contenteditable attribute do in HTML?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Allows a user to upload content</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Makes the element read-only</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Allows the user to edit the content in place</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Embeds rich content like video</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>What is the specificity of this selector: div#main.content &gt; p.intro?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1-1-2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0-2-2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1-2-2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1-1-1</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>What CSS property prevents an element from being resized by the user in a textarea?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>resize: none;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>overflow: hidden;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>user-select: none;</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>pointer-events: none;</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>What does z-index apply to?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Static elements</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>All elements</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Positioned elements(relative, absolute, fixed, sticky)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Only flex containers</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>What is the default value of the CSS position property</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>relative</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>abolute</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>inherit</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Which of the following units is relative to the viewport width?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>em</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vh</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>rem</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>vw</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>What HTML tag is used for defining a document's navigation links?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>&lt;nav&gt;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>&lt;link&gt;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>&lt;menu&gt;</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>&lt;aside&gt;</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Which of the following is not a semantic HTML5 element?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>&lt;section&gt;</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>&lt;article&gt;</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>&lt;header&gt;</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>What does the defer attribute do on a script tag?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Executes the script immediately</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Executes the script after DOM is parsed</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Delays loading until window.onload</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Ignores script execution</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Which CSS property helps with performance in hardware-accelerated animations</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>transform</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>width</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>opacity</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing Categories and Quiz
</commit_message>
<xml_diff>
--- a/quizzes.xlsx
+++ b/quizzes.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Web Development 1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Python 1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Python 3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Web Development 3" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Cryptography 1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="General 2" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="General 3" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Python 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Python 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Web Development 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="General 2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="General 1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="General 3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Web Development 1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Cryptography 1" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -438,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,134 +450,134 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Web Development 1</t>
+          <t>Python 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>Python</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>What does HTML stand for?</t>
+          <t>How do you print something in Python?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hyperlink Markup Language</t>
+          <t>echo()</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HyperText Markup Language</t>
+          <t>printf()</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>HyperTransfer Markup Language</t>
+          <t>print()</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>None of the above</t>
+          <t>show()</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Which tag is used to create a hyperlink in HTML?</t>
+          <t>What is the correct syntax to assign a variable in Python?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>&lt;a&gt;</t>
+          <t>x := 5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>&lt;link&gt;</t>
+          <t>x == 5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>&lt;href&gt;</t>
+          <t>x = 5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>&lt;hyper&gt;</t>
+          <t>let x = 5</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What is CSS used for?</t>
+          <t>What does the len() function do?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adding behavior to elements</t>
+          <t>Returns the memory address</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Creating databases</t>
+          <t>Returns the length of an object</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Styling HTML elements</t>
+          <t>Lists environment variables</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Structuring content</t>
+          <t>Encrypts strings</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>What is the default method for submitting a form in HTML?</t>
+          <t>What is a correct way to define a function in Python?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>function myFunc():</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>def myFunc():</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>func myFunc():</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>FETCH</t>
+          <t>define myFunc():</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -586,181 +587,157 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Which HTTP status code means “Not Found”?</t>
+          <t>What is a Python list?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>A key-value pair structure</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>An immutable collection</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>A mutable ordered sequence</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>A fixed-size array</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Which JavaScript keyword is used to declare a constant?</t>
+          <t>Which keyword handles exceptions?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>let</t>
+          <t>except</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>var</t>
+          <t>raise</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>const</t>
+          <t>throw</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>define</t>
+          <t>trap</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>What does AJAX stand for?</t>
+          <t>What is a lambda function?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Asynchronous JavaScript and XML</t>
+          <t>A function declared with def</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Advanced JSON and XML</t>
+          <t>A built-in exception</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Application JavaScript and XHTML</t>
+          <t>An anonymous function expressed as a single line</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Asynchronous JSON Access Exchange</t>
+          <t>A loop structure</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Which of the following is a frontend framework?</t>
+          <t>What is the output of the following code?
+ python
+CopyEdit
+x = [1, 2, 3]
+y = x
+y.append(4)
+print(x)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Django</t>
+          <t>[1, 2, 3]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Flask</t>
+          <t>[1, 2, 3, 4]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>React</t>
+          <t>[4, 1, 2, 3]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Express</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>In RESTful APIs, which HTTP method is typically used for updates?</t>
+          <t>What is a Python decorator used for?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>Styling code</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>Running scripts in parallel</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>Modifying or enhancing functions or methods</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>HEAD</t>
+          <t>Defining variables inside a class</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>What does the “Content Security Policy” header do?</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Prevents SQL injection</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Restricts resources the browser is allowed to load</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Blocks spam bots</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Enforces data encryption</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -774,7 +751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,12 +762,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Python 1</t>
+          <t>Python 3</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -802,27 +779,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>How do you print something in Python?</t>
+          <t>What does the @classmethod decorator do?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>echo()</t>
+          <t>Converts a method into a static method</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>printf()</t>
+          <t>Converts a method so it can only be called on class instances</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>print()</t>
+          <t>Converts a method to receive the class as the first argument instead of the instance</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>show()</t>
+          <t>Makes the method private</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -832,27 +809,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>What is the correct syntax to assign a variable in Python?</t>
+          <t>Which of the following statements is TRUE about Python’s GIL (Global Interpreter Lock)?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>x := 5</t>
+          <t>It allows true parallel execution of threads on multiple CPUs</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>x == 5</t>
+          <t>It prevents memory leaks in C extensions</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>x = 5</t>
+          <t>It ensures only one thread executes Python bytecode at a time</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>let x = 5</t>
+          <t>It is removed in Python 3.10</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -862,87 +839,87 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What does the len() function do?</t>
+          <t>How can you create a custom context manager in Python?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Returns the memory address</t>
+          <t>Using @classmethod</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Returns the length of an object</t>
+          <t>Using __init__ and __del__</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Lists environment variables</t>
+          <t>By defining __enter__ and __exit__ methods</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Encrypts strings</t>
+          <t>By using yield without any decorators</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>What is a correct way to define a function in Python?</t>
+          <t>Which of the following is used to define an abstract method in Python?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>function myFunc():</t>
+          <t>from abc import abstractmethod</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>def myFunc():</t>
+          <t>@abstractmethod</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>func myFunc():</t>
+          <t>def method(self): pass</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>define myFunc():</t>
+          <t>Both A and B</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What is a Python list?</t>
+          <t>What is the primary purpose of __slots__ in a class?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A key-value pair structure</t>
+          <t>To define class-level constants</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>An immutable collection</t>
+          <t>To create a dictionary for instance variables</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>A mutable ordered sequence</t>
+          <t>To prevent dynamic creation of new attributes and reduce memory</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>A fixed-size array</t>
+          <t>To define abstract methods</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -952,57 +929,57 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Which keyword handles exceptions?</t>
+          <t>Which statement is true about Python descriptors?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>except</t>
+          <t>They only work with class methods</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>raise</t>
+          <t>They define attribute access using __get__, __set__, __delete__</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>throw</t>
+          <t>Descriptors are only available in Python 3.10+</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>trap</t>
+          <t>Descriptors cannot be reused across classes</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>What is a lambda function?</t>
+          <t>What is a coroutine in Python?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A function declared with def</t>
+          <t>A thread</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A built-in exception</t>
+          <t>A class with __iter__</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>An anonymous function expressed as a single line</t>
+          <t>a function paused with yield and resumed later</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>A loop structure</t>
+          <t>A method in a metaclass</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -1012,67 +989,91 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>What is the output of the following code?
- python
-CopyEdit
-x = [1, 2, 3]
-y = x
-y.append(4)
-print(x)</t>
+          <t>Which of the following is not a valid use of a metaclass?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[1, 2, 3]</t>
+          <t>Injecting methods into a class</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[1, 2, 3, 4]</t>
+          <t>Enforcing naming conventions</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[4, 1, 2, 3]</t>
+          <t>Changing inheritance at runtime</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Error</t>
+          <t>Dynamically creating instance variables</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>What is a Python decorator used for?</t>
+          <t>What does weakref module provide in Python?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Styling code</t>
+          <t>Multithreading support</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Running scripts in parallel</t>
+          <t>References that do not increase reference count</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Modifying or enhancing functions or methods</t>
+          <t>Dynamic type checking</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Defining variables inside a class</t>
+          <t>Object pooling</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>What does the super() function do in Python?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Calls a method from a subclass</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Calls the next method in the method resolution order (MRO)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Creates a static method</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Returns the parent class constructor  directly</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1098,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Python 3</t>
+          <t>Web Development 3</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1107,34 +1108,34 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Web Development</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>What does the @classmethod decorator do?</t>
+          <t>What does the contenteditable attribute do in HTML?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Converts a method into a static method</t>
+          <t>Allows a user to upload content</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Converts a method so it can only be called on class instances</t>
+          <t>Makes the element read-only</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Converts a method to receive the class as the first argument instead of the instance</t>
+          <t>Allows the user to edit the content in place</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Makes the method private</t>
+          <t>Embeds rich content like video</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -1144,57 +1145,57 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Which of the following statements is TRUE about Python’s GIL (Global Interpreter Lock)?</t>
+          <t>What is the specificity of this selector: div#main.content &gt; p.intro?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>It allows true parallel execution of threads on multiple CPUs</t>
+          <t>1-1-2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>It prevents memory leaks in C extensions</t>
+          <t>0-2-2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>It ensures only one thread executes Python bytecode at a time</t>
+          <t>1-2-2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>It is removed in Python 3.10</t>
+          <t>1-1-1</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>How can you create a custom context manager in Python?</t>
+          <t>What CSS property prevents an element from being resized by the user in a textarea?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Using @classmethod</t>
+          <t>resize: none;</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Using __init__ and __del__</t>
+          <t>overflow: hidden;</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>By defining __enter__ and __exit__ methods</t>
+          <t>user-select: none;</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>By using yield without any decorators</t>
+          <t>pointer-events: none;</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -1204,177 +1205,177 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Which of the following is used to define an abstract method in Python?</t>
+          <t>What does z-index apply to?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>from abc import abstractmethod</t>
+          <t>Static elements</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>@abstractmethod</t>
+          <t>All elements</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>def method(self): pass</t>
+          <t>Positioned elements(relative, absolute, fixed, sticky)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Both A and B</t>
+          <t>Only flex containers</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What is the primary purpose of __slots__ in a class?</t>
+          <t>What is the default value of the CSS position property</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>To define class-level constants</t>
+          <t>relative</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>To create a dictionary for instance variables</t>
+          <t>static</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>To prevent dynamic creation of new attributes and reduce memory</t>
+          <t>abolute</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>To define abstract methods</t>
+          <t>inherit</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Which statement is true about Python descriptors?</t>
+          <t>Which of the following units is relative to the viewport width?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>They only work with class methods</t>
+          <t>em</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>They define attribute access using __get__, __set__, __delete__</t>
+          <t>vh</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Descriptors are only available in Python 3.10+</t>
+          <t>rem</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Descriptors cannot be reused across classes</t>
+          <t>vw</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>What is a coroutine in Python?</t>
+          <t>What HTML tag is used for defining a document's navigation links?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A thread</t>
+          <t>&lt;nav&gt;</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A class with __iter__</t>
+          <t>&lt;link&gt;</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>a function paused with yield and resumed later</t>
+          <t>&lt;menu&gt;</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>A method in a metaclass</t>
+          <t>&lt;aside&gt;</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Which of the following is not a valid use of a metaclass?</t>
+          <t>Which of the following is not a semantic HTML5 element?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Injecting methods into a class</t>
+          <t>&lt;section&gt;</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Enforcing naming conventions</t>
+          <t>&lt;article&gt;</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Changing inheritance at runtime</t>
+          <t>&lt;div&gt;</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Dynamically creating instance variables</t>
+          <t>&lt;header&gt;</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>What does weakref module provide in Python?</t>
+          <t>What does the defer attribute do on a script tag?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Multithreading support</t>
+          <t>Executes the script immediately</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>References that do not increase reference count</t>
+          <t>Executes the script after DOM is parsed</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dynamic type checking</t>
+          <t>Delays loading until window.onload</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Object pooling</t>
+          <t>Ignores script execution</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1384,31 +1385,31 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>What does the super() function do in Python?</t>
+          <t>Which CSS property helps with performance in hardware-accelerated animations</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Calls a method from a subclass</t>
+          <t>transform</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Calls the next method in the method resolution order (MRO)</t>
+          <t>top</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Creates a static method</t>
+          <t>width</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Returns the parent class constructor  directly</t>
+          <t>opacity</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1417,6 +1418,72 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>General 2</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What is part of a database that holds only one type of information?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Record</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Report</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>file</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Field</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1433,164 +1500,164 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Web Development 3</t>
+          <t>General 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>General</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>What does the contenteditable attribute do in HTML?</t>
+          <t>What does CPU stand for?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Allows a user to upload content</t>
+          <t>Central Process Unit</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Makes the element read-only</t>
+          <t>Central Processing Unit</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Allows the user to edit the content in place</t>
+          <t>Computer Processing Unit</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Embeds rich content like video</t>
+          <t>Central Peripheral Unit</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>What is the specificity of this selector: div#main.content &gt; p.intro?</t>
+          <t>What is the shortcut for copying text on most computers?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1-1-2</t>
+          <t>Ctrl + V</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0-2-2</t>
+          <t>Ctrl + C</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1-2-2</t>
+          <t>Ctrl + X</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1-1-1</t>
+          <t>Ctrl + Z</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What CSS property prevents an element from being resized by the user in a textarea?</t>
+          <t>Which of these file types is a compressed archive?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>resize: none;</t>
+          <t>.docx</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>overflow: hidden;</t>
+          <t>.zip</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>user-select: none;</t>
+          <t>.exe</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>pointer-events: none;</t>
+          <t>.txt</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>What does z-index apply to?</t>
+          <t>What does DNS stand for?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Static elements</t>
+          <t>Digital Network System</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>All elements</t>
+          <t>Domain Name System</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Positioned elements(relative, absolute, fixed, sticky)</t>
+          <t>Distributed Name Service</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Only flex containers</t>
+          <t>Domain Network Service</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What is the default value of the CSS position property</t>
+          <t>What does “ping” do in networking?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>relative</t>
+          <t>Encrypts data</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>static</t>
+          <t>Sends a test packet to check connectivity</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>abolute</t>
+          <t>Installs software</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>inherit</t>
+          <t>Tracks location</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -1600,87 +1667,87 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Which of the following units is relative to the viewport width?</t>
+          <t>Which command shows all active network connections in Windows?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>em</t>
+          <t>ipconfig</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>vh</t>
+          <t>netstat</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>rem</t>
+          <t>traceroute</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>vw</t>
+          <t>ping</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>What HTML tag is used for defining a document's navigation links?</t>
+          <t>What does the acronym API stand for?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>&lt;nav&gt;</t>
+          <t>Automatic Program Interface</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>&lt;link&gt;</t>
+          <t>Application Programming Interface</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>&lt;menu&gt;</t>
+          <t>Advanced Protocol Interface</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>&lt;aside&gt;</t>
+          <t>Applied Programming Integration</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Which of the following is not a semantic HTML5 element?</t>
+          <t>Which port does HTTPS typically use?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>&lt;section&gt;</t>
+          <t>80</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>&lt;article&gt;</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>&lt;div&gt;</t>
+          <t>443</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>&lt;header&gt;</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1690,276 +1757,60 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>What does the defer attribute do on a script tag?</t>
+          <t>What is a “man-in-the-middle” attack?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Executes the script immediately</t>
+          <t>A firewall misconfiguration</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Executes the script after DOM is parsed</t>
+          <t>A user stealing Wi-Fi</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Delays loading until window.onload</t>
+          <t>An attacker intercepting communication between two parties</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Ignores script execution</t>
+          <t>A broken DNS record</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Which CSS property helps with performance in hardware-accelerated animations</t>
+          <t>What is the purpose of the OSI model in networking?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>transform</t>
+          <t>To define a universal coding language</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>top</t>
+          <t>To explain layers of software development</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>width</t>
+          <t>To standardize network communication into layers</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>opacity</t>
+          <t>To test system security</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Cryptography 1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Encryption</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Cryptography</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Which algorithm is considered broken due to short key length?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AES</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>DES</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Blowfish</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RSA-2048</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>What is the size of an SHA-256 hash?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>64 bits</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>128 bits</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>256 bits</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>512 bits</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>What kind of cryptography uses two different keys?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Symmetric</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Asymmetric</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Elliptic</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Hashing</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>What does a digital signature ensure?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Faster loading</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Data authenticity and integrity</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Confidentiality only</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Compression of data</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>What is “salting” in password hashing?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Encrypting passwords</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Adding a secret value before hashing to prevent rainbow table attacks</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Encoding data into Base64</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Decrypting a stored password</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Which algorithm is commonly used in blockchain for proof-of-work?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>RSA</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MD5</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>SHA-256</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>HMAC</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1974,7 +1825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1985,12 +1836,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>General 2</t>
+          <t>General 3</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Recycle Bin</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -2002,91 +1853,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>You receive a file with a .xlsx extension. Which type of software is most appropriate to open and edit this file?</t>
+          <t>The speed of your net access is defined in terms of...</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Word Processor</t>
+          <t>RAM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Spreadsheet Application</t>
+          <t>MHz</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Presentation Software</t>
+          <t>Kbps</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Database Management Systemn cybersecurity, what is phishing?</t>
+          <t>Megabytes</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>In cybersecurity, what is phishing?</t>
+          <t>How many diodes are in a full wave bridge rectifier?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A method of testing server speed</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A type of email scam</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>A computer virus</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A way to improve internet performance</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>What is part of a database that holds only one type of information?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Record</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Report</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>file</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Field</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2095,6 +1916,282 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Web Development 1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Web Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What is CSS used for?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Adding behavior to elements</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Creating databases</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Styling HTML elements</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Structuring content</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>What is the default method for submitting a form in HTML?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FETCH</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Which HTTP status code means “Not Found”?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>403</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>404</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Which JavaScript keyword is used to declare a constant?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>let</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>var</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>const</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>define</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>What does AJAX stand for?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Asynchronous JavaScript and XML</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Advanced JSON and XML</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Application JavaScript and XHTML</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Asynchronous JSON Access Exchange</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Which of the following is a frontend framework?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Django</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Flask</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>React</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>In RESTful APIs, which HTTP method is typically used for updates?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>PUT</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DELETE</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>HEAD</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>What does the “Content Security Policy” header do?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Prevents SQL injection</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Restricts resources the browser is allowed to load</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Blocks spam bots</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Enforces data encryption</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2111,134 +2208,134 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>General 3</t>
+          <t>Cryptography 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Contact your Internet service provider</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Cryptography</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Computers calculate numbers in what mode?</t>
+          <t>What kind of cryptography uses two different keys?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Decimal</t>
+          <t>Symmetric</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Octal</t>
+          <t>Asymmetric</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Binary</t>
+          <t>Elliptic</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>None of the above</t>
+          <t>Hashing</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>What is an FET?</t>
+          <t>What does a digital signature ensure?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Farad Effect Transformer</t>
+          <t>Faster loading</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Field Effect Transformer</t>
+          <t>Data authenticity and integrity</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Field Effect Transistor</t>
+          <t>Confidentiality only</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>French Energy Transfer</t>
+          <t>Compression of data</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>The speed of your net access is defined in terms of...</t>
+          <t>What is “salting” in password hashing?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RAM</t>
+          <t>Encrypting passwords</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MHz</t>
+          <t>Adding a secret value before hashing to prevent rainbow table attacks</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Kbps</t>
+          <t>Encoding data into Base64</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Megabytes</t>
+          <t>Decrypting a stored password</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>How many diodes are in a full wave bridge rectifier?</t>
+          <t>Which algorithm is commonly used in blockchain for proof-of-work?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>RSA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>SHA-256</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>HMAC</t>
         </is>
       </c>
       <c r="F5" t="n">

</xml_diff>